<commit_message>
20190531 last commited sekkeisho
</commit_message>
<xml_diff>
--- a/設計書/NewsScrapingforSlack.xlsx
+++ b/設計書/NewsScrapingforSlack.xlsx
@@ -4623,8 +4623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89:D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>

</xml_diff>